<commit_message>
Status translation & postal lookup
</commit_message>
<xml_diff>
--- a/src/test/resources/GER.test.xlsx
+++ b/src/test/resources/GER.test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="JE" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="80">
   <si>
     <t xml:space="preserve">GERNR</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve">Test road 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3900 Nuuk</t>
   </si>
   <si>
     <t xml:space="preserve">person@example.com</t>
@@ -278,7 +275,7 @@
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -300,12 +297,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -363,7 +354,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,32 +385,32 @@
   </sheetPr>
   <dimension ref="A1:AP65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="7" min="4" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="40.919028340081"/>
     <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="25" min="15" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="28" min="28" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="28.1740890688259"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="28.3846153846154"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="32" min="32" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="37" min="35" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="38" min="38" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="39" style="0" width="8.57085020242915"/>
@@ -569,11 +560,8 @@
       <c r="H2" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="0" t="s">
-        <v>46</v>
-      </c>
       <c r="M2" s="0" t="n">
-        <v>3900</v>
+        <v>3982</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>6</v>
@@ -591,16 +579,16 @@
         <v>123456</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="W2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="Y2" s="1" t="n">
         <v>432200</v>
@@ -610,7 +598,7 @@
       </c>
       <c r="AA2" s="2"/>
       <c r="AC2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AD2" s="2" t="n">
         <v>40767</v>
@@ -619,16 +607,16 @@
         <v>43008</v>
       </c>
       <c r="AF2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG2" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="AH2" s="2" t="n">
         <v>43089</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4066,18 +4054,18 @@
   </sheetPr>
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.6720647773279"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4092,22 +4080,22 @@
         <v>22</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="H1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>2</v>
@@ -4143,7 +4131,7 @@
         <v>12</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V1" s="0" t="s">
         <v>14</v>
@@ -4179,7 +4167,7 @@
         <v>26</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AH1" s="0" t="s">
         <v>28</v>
@@ -4194,7 +4182,7 @@
         <v>31</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4205,38 +4193,38 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234567890</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>42</v>
       </c>
       <c r="I2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>44</v>
       </c>
       <c r="O2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="S2" s="0" t="n">
         <v>42</v>
@@ -4273,7 +4261,7 @@
         <v>41897</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AH2" s="1"/>
       <c r="AI2" s="2" t="n">
@@ -4283,7 +4271,7 @@
         <v>43089</v>
       </c>
       <c r="AK2" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -4312,20 +4300,20 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9595141700405"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.5627530364373"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4340,43 +4328,43 @@
         <v>22</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="M1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4387,7 +4375,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2"/>
       <c r="F2" s="2" t="n">
@@ -4401,13 +4389,13 @@
         <v>43101</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>123456789</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>1234567890</v>
@@ -4440,7 +4428,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>